<commit_message>
RAB-1589: Family templates generator should handle family title
</commit_message>
<xml_diff>
--- a/tests/Command/GenerateTemplatesCommand/source_file.xlsx
+++ b/tests/Command/GenerateTemplatesCommand/source_file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14340" windowHeight="14190" activeTab="1"/>
+    <workbookView windowWidth="14340" windowHeight="12195" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Industries" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="188">
   <si>
     <t>code</t>
   </si>
@@ -466,22 +466,28 @@
     <t>Oversized</t>
   </si>
   <si>
-    <t>family</t>
-  </si>
-  <si>
     <t>description-en_US</t>
   </si>
   <si>
     <t>videogames</t>
   </si>
   <si>
+    <t>Videogames</t>
+  </si>
+  <si>
     <t>Embark on epic adventures with our 'Videogames' family template - an immersive collection of pre-built attributes to seamlessly manage your gaming essentials, unlocking a world of entertainment and excitement.</t>
   </si>
   <si>
+    <t>Jerseys</t>
+  </si>
+  <si>
     <t>Cheer on your favorite teams with our 'Jerseys' family template - a winning assortment of pre-built attributes to easily manage your sports apparel, showing your team spirit in style.</t>
   </si>
   <si>
     <t>headphones</t>
+  </si>
+  <si>
+    <t>Headphones</t>
   </si>
   <si>
     <t>Immerse yourself in sound with our 'Headphones' family template - a premium assortment of pre-built attributes to manage your audio companions, delivering a personal concert experience wherever you go.</t>
@@ -660,10 +666,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -710,21 +716,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -733,10 +724,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -755,6 +777,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -765,30 +794,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -802,21 +808,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -824,7 +816,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -839,7 +831,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -847,17 +847,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -881,7 +887,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -893,13 +899,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,25 +941,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -941,109 +959,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,6 +984,84 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,6 +1090,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1095,15 +1136,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1127,22 +1159,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1155,162 +1172,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1678,7 +1684,7 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
@@ -2304,56 +2310,69 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="21.247619047619" customWidth="1"/>
-    <col min="2" max="2" width="109" customWidth="1"/>
+    <col min="1" max="2" width="21.247619047619" customWidth="1"/>
+    <col min="3" max="3" width="109" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" customHeight="1" spans="1:3">
       <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="15" t="s">
+    </row>
+    <row r="2" customHeight="1" spans="1:3">
+      <c r="A2" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:2">
-      <c r="A2" s="16" t="s">
+      <c r="B2" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:2">
+    <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:2">
+      <c r="C3" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="17" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:1">
+      <c r="B4" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:2">
       <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="_x0001_" sqref="B2 B3 B4">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="_x0001_" sqref="C2 C3 C4">
       <formula1>LEN(#REF!)&lt;255</formula1>
     </dataValidation>
   </dataValidations>
@@ -2393,33 +2412,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D2" s="10">
         <v>0</v>
@@ -2428,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12">
@@ -2437,13 +2456,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -2452,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="10">
@@ -2464,10 +2483,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D4" s="10">
         <v>0</v>
@@ -2476,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="10">
@@ -2485,13 +2504,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D5" s="10">
         <v>0</v>
@@ -2500,7 +2519,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="10">
@@ -2509,13 +2528,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -2524,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="10">
@@ -2533,13 +2552,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D7" s="10">
         <v>0</v>
@@ -2548,10 +2567,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H7" s="10">
         <v>0</v>
@@ -2562,10 +2581,10 @@
         <v>45</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D8" s="10">
         <v>0</v>
@@ -2574,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="10">
@@ -2586,10 +2605,10 @@
         <v>56</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D9" s="10">
         <v>0</v>
@@ -2598,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="10">
@@ -2610,11 +2629,11 @@
         <v>67</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
         <v>158</v>
       </c>
-      <c r="C10" t="s">
-        <v>156</v>
-      </c>
       <c r="D10" s="10">
         <v>0</v>
       </c>
@@ -2622,7 +2641,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="10">
@@ -2634,10 +2653,10 @@
         <v>78</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D11" s="10">
         <v>0</v>
@@ -2646,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="10">
@@ -2658,10 +2677,10 @@
         <v>100</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -2670,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="10">
@@ -2714,33 +2733,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -2749,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -2758,13 +2777,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -2773,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -2782,13 +2801,13 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -2797,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
@@ -2806,13 +2825,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -2821,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="3">
@@ -2830,13 +2849,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -2845,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3">
@@ -2854,13 +2873,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -2869,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="3">
@@ -2878,13 +2897,13 @@
     </row>
     <row r="8" customHeight="1" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -2893,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H8" s="4">
         <v>0</v>
@@ -2904,25 +2923,25 @@
     </row>
     <row r="9" customHeight="1" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="H9" s="4">
         <v>0</v>
@@ -2930,13 +2949,13 @@
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -2945,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4">
@@ -2954,13 +2973,13 @@
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -2969,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
@@ -3013,33 +3032,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -3048,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -3057,13 +3076,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -3072,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -3081,13 +3100,13 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -3096,7 +3115,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="3">
@@ -3105,13 +3124,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -3120,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="3">
@@ -3129,13 +3148,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -3144,7 +3163,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3">
@@ -3156,10 +3175,10 @@
         <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -3168,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3">
@@ -3180,10 +3199,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -3192,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="3">
@@ -3204,10 +3223,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -3216,7 +3235,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3">
@@ -3228,10 +3247,10 @@
         <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -3240,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="3">

</xml_diff>

<commit_message>
RAB-1480: Force type string
</commit_message>
<xml_diff>
--- a/tests/Command/GenerateTemplatesCommand/source_file.xlsx
+++ b/tests/Command/GenerateTemplatesCommand/source_file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14340" windowHeight="12195" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="14370" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Industries" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="191">
   <si>
     <t>code</t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>Playstation 5</t>
+  </si>
+  <si>
+    <t>platform6</t>
+  </si>
+  <si>
+    <t>platform7</t>
+  </si>
+  <si>
+    <t>1-2</t>
   </si>
   <si>
     <t>video_game_genre1</t>
@@ -717,8 +726,84 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,7 +818,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,47 +838,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -807,61 +868,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -887,7 +896,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,31 +920,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,97 +938,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,7 +962,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1055,13 +992,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1072,6 +1081,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1094,18 +1112,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1125,17 +1156,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1154,173 +1181,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1363,6 +1372,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1682,12 +1692,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="2"/>
@@ -2042,242 +2052,254 @@
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>77</v>
+      <c r="B32" s="18">
+        <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:3">
       <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:3">
       <c r="A35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:3">
       <c r="A36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:3">
       <c r="A37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="1:3">
       <c r="A39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="40" customHeight="1" spans="1:3">
       <c r="A40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:3">
       <c r="A41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="1:3">
       <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" customHeight="1" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" customHeight="1" spans="1:3">
       <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="45" customHeight="1" spans="1:3">
       <c r="A45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" customHeight="1" spans="1:3">
       <c r="A46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:3">
       <c r="A48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="1:3">
       <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" customHeight="1" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:3">
       <c r="A51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="52" customHeight="1" spans="1:3">
       <c r="A52" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="C52" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" customHeight="1" spans="1:3">
+      <c r="A53" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" customHeight="1" spans="1:3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="1"/>
+      <c r="B53" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="54" customHeight="1" spans="1:3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="55" customHeight="1" spans="1:3">
       <c r="A55" s="1"/>
@@ -2298,6 +2320,16 @@
       <c r="A58" s="1"/>
       <c r="B58" s="7"/>
       <c r="C58" s="1"/>
+    </row>
+    <row r="59" customHeight="1" spans="1:3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" customHeight="1" spans="1:3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2312,7 +2344,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2330,18 +2362,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="16" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
@@ -2349,21 +2381,21 @@
         <v>8</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:2">
@@ -2412,33 +2444,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D2" s="10">
         <v>0</v>
@@ -2447,7 +2479,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12">
@@ -2456,13 +2488,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -2471,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="10">
@@ -2483,10 +2515,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D4" s="10">
         <v>0</v>
@@ -2495,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="10">
@@ -2504,13 +2536,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D5" s="10">
         <v>0</v>
@@ -2519,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="10">
@@ -2528,13 +2560,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -2543,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="10">
@@ -2552,13 +2584,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D7" s="10">
         <v>0</v>
@@ -2567,10 +2599,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H7" s="10">
         <v>0</v>
@@ -2581,10 +2613,10 @@
         <v>45</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D8" s="10">
         <v>0</v>
@@ -2593,7 +2625,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="10">
@@ -2605,10 +2637,10 @@
         <v>56</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D9" s="10">
         <v>0</v>
@@ -2617,7 +2649,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="10">
@@ -2629,10 +2661,10 @@
         <v>67</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D10" s="10">
         <v>0</v>
@@ -2641,7 +2673,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="10">
@@ -2650,14 +2682,14 @@
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" t="s">
         <v>161</v>
       </c>
-      <c r="C11" t="s">
-        <v>158</v>
-      </c>
       <c r="D11" s="10">
         <v>0</v>
       </c>
@@ -2665,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="10">
@@ -2674,13 +2706,13 @@
     </row>
     <row r="12" customHeight="1" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -2689,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="10">
@@ -2733,33 +2765,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -2768,7 +2800,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -2777,13 +2809,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -2792,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -2801,13 +2833,13 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -2816,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3">
@@ -2825,13 +2857,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -2840,7 +2872,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="3">
@@ -2849,13 +2881,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -2864,7 +2896,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3">
@@ -2873,13 +2905,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -2888,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="3">
@@ -2897,13 +2929,13 @@
     </row>
     <row r="8" customHeight="1" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -2912,10 +2944,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H8" s="4">
         <v>0</v>
@@ -2923,13 +2955,13 @@
     </row>
     <row r="9" customHeight="1" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -2938,10 +2970,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H9" s="4">
         <v>0</v>
@@ -2949,13 +2981,13 @@
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -2964,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4">
@@ -2973,13 +3005,13 @@
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -2988,7 +3020,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
@@ -3032,33 +3064,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -3067,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3">
@@ -3076,13 +3108,13 @@
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -3091,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
@@ -3100,13 +3132,13 @@
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -3115,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="3">
@@ -3124,13 +3156,13 @@
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -3139,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="3">
@@ -3148,13 +3180,13 @@
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -3163,7 +3195,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3">
@@ -3172,13 +3204,13 @@
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -3187,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3">
@@ -3199,10 +3231,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -3211,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="3">
@@ -3223,10 +3255,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -3235,7 +3267,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3">
@@ -3244,13 +3276,13 @@
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -3259,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="3">

</xml_diff>

<commit_message>
RAB-1824: add validation rule property foreach text attribute
</commit_message>
<xml_diff>
--- a/tests/Command/GenerateTemplatesCommand/source_file.xlsx
+++ b/tests/Command/GenerateTemplatesCommand/source_file.xlsx
@@ -4,7 +4,7 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Industries" sheetId="1" state="visible" r:id="rId2"/>
@@ -545,6 +545,12 @@
     <t>type</t>
   </si>
   <si>
+    <t>attribute_group</t>
+  </si>
+  <si>
+    <t>validation_rule</t>
+  </si>
+  <si>
     <t>scopable</t>
   </si>
   <si>
@@ -578,6 +584,9 @@
     <t>pim_catalog_identifier</t>
   </si>
   <si>
+    <t>other</t>
+  </si>
+  <si>
     <t>template</t>
   </si>
   <si>
@@ -711,15 +720,6 @@
   </si>
   <si>
     <t>Cut</t>
-  </si>
-  <si>
-    <t>attribute_group</t>
-  </si>
-  <si>
-    <t>validation_rule</t>
-  </si>
-  <si>
-    <t>other</t>
   </si>
   <si>
     <t>eu_declaration_of_conformity</t>
@@ -913,12 +913,14 @@
       <alignment vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -970,7 +972,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{2265CD29-3746-8DB5-7BD6-88BCB7AB78A2}"/>
+  <person displayName=" " id="{BC36CD6E-B780-8099-B33A-D6EAA0A89997}"/>
 </personList>
 </file>
 
@@ -1430,7 +1432,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" personId="{2265CD29-3746-8DB5-7BD6-88BCB7AB78A2}" id="{00190023-0011-4759-8904-001F003A0020}" done="0">
+  <threadedComment ref="A1" personId="{BC36CD6E-B780-8099-B33A-D6EAA0A89997}" id="{00190023-0011-4759-8904-001F003A0020}" done="0">
     <text xml:space="preserve">Tires are so complicated. Variant are under at least 3 levels of variation "height, width, diameter, charge indice". It is a pitfall here.
 -Nelly Devaine
 ----
@@ -2301,19 +2303,19 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2325,7 +2327,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00750073-006B-478B-8F50-00BE00B50022}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="_x0001_" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004F0023-0092-4041-B8C8-006C00A600E5}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="_x0001_" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(#ref!)&lt;255</xm:f>
           </x14:formula1>
@@ -2334,13 +2336,13 @@
           </x14:formula2>
           <xm:sqref>E2:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00E000DF-0039-458E-A99B-0094005F0020}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000400A8-004B-4CFD-A5A3-004B001C000F}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(C16)&lt;255</xm:f>
           </x14:formula1>
           <xm:sqref>C5:D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00230011-0045-4495-9EE0-00B000ED0007}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00B70015-0050-47AE-919B-008800DA00AB}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(B16)&lt;255</xm:f>
           </x14:formula1>
@@ -2368,10 +2370,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="28.760000000000002"/>
     <col customWidth="1" min="2" max="2" style="1" width="20.629999999999999"/>
-    <col customWidth="1" min="3" max="3" style="1" width="23.5"/>
-    <col customWidth="1" min="4" max="6" style="1" width="12.380000000000001"/>
-    <col customWidth="1" min="7" max="7" style="1" width="13.5"/>
-    <col customWidth="1" min="8" max="11" style="1" width="13.24"/>
+    <col customWidth="1" min="3" max="5" style="1" width="23.5"/>
+    <col customWidth="1" min="6" max="8" style="1" width="12.380000000000001"/>
+    <col customWidth="1" min="9" max="9" style="1" width="13.5"/>
+    <col customWidth="1" min="10" max="13" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2408,31 +2410,41 @@
       <c r="K1" s="2" t="s">
         <v>153</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="13">
-        <v>0</v>
-      </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+        <v>158</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="15">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2440,26 +2452,30 @@
       <c r="A3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>158</v>
+      <c r="B3" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="13">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="E3" s="1"/>
+      <c r="F3" s="13">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="13">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2467,26 +2483,30 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="13">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="13">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="13">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2494,84 +2514,96 @@
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>162</v>
+      <c r="B5" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+        <v>166</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="13">
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="13">
-        <v>0</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+        <v>169</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="13">
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>170</v>
+        <v>172</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="13">
+        <v>0</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="13">
+        <v>160</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2580,25 +2612,29 @@
         <v>48</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+        <v>176</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="13">
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2607,25 +2643,29 @@
         <v>59</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="13">
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="13">
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2634,25 +2674,29 @@
         <v>70</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="13">
-        <v>0</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+        <v>176</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="13">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2661,25 +2705,29 @@
         <v>84</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="D11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="13">
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="13">
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2688,54 +2736,62 @@
         <v>106</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="13">
+        <v>0</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="13">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="13" ht="12.800000000000001">
       <c r="A13" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="I13" s="1">
+        <v>183</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="K13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2763,10 +2819,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="28.760000000000002"/>
     <col customWidth="1" min="2" max="2" style="1" width="20.629999999999999"/>
-    <col customWidth="1" min="3" max="3" style="1" width="22.379999999999999"/>
-    <col customWidth="1" min="4" max="6" style="1" width="12.380000000000001"/>
-    <col customWidth="1" min="7" max="7" style="1" width="13.5"/>
-    <col customWidth="1" min="8" max="11" style="1" width="13.24"/>
+    <col customWidth="1" min="3" max="5" style="1" width="22.379999999999999"/>
+    <col customWidth="1" min="6" max="8" style="1" width="12.380000000000001"/>
+    <col customWidth="1" min="9" max="9" style="1" width="13.5"/>
+    <col customWidth="1" min="10" max="13" style="1" width="13.24"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2779,10 +2835,10 @@
       <c r="C1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>147</v>
       </c>
       <c r="F1" s="14" t="s">
@@ -2794,67 +2850,81 @@
       <c r="H1" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="2" t="s">
         <v>153</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+        <v>158</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="14">
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+        <v>183</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="14">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2862,53 +2932,61 @@
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>158</v>
+      <c r="B4" s="11" t="s">
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="E4" s="1"/>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="H4" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-      <c r="K4" s="14">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>182</v>
+        <v>184</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
+        <v>186</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
         <v>1</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="14">
+      <c r="H5" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2916,26 +2994,30 @@
       <c r="A6" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>162</v>
+      <c r="B6" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+        <v>166</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="14">
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2943,150 +3025,170 @@
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>184</v>
+      <c r="B7" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="14">
+        <v>166</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>0</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>187</v>
+        <v>172</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="I8" s="14">
+        <v>160</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" s="14">
         <v>1</v>
       </c>
-      <c r="J8" s="14">
-        <v>0</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="I9" s="14">
+      <c r="J9" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="K9" s="14">
         <v>1</v>
       </c>
-      <c r="J9" s="14">
-        <v>0</v>
-      </c>
-      <c r="K9" s="14">
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+        <v>169</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="14">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+        <v>169</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14">
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3105,7 +3207,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" zoomScale="55" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A3" zoomScale="55" workbookViewId="0">
       <selection activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -3113,12 +3215,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="24.629999999999999"/>
     <col customWidth="1" min="2" max="2" style="1" width="24.760000000000002"/>
-    <col customWidth="1" min="3" max="3" style="1" width="23.629999999999999"/>
-    <col customWidth="1" min="4" max="4" style="1" width="12"/>
-    <col customWidth="1" min="5" max="5" style="1" width="12.24"/>
+    <col customWidth="1" min="3" max="5" style="1" width="23.629999999999999"/>
     <col customWidth="1" min="6" max="6" style="1" width="12"/>
-    <col customWidth="1" min="7" max="7" style="1" width="12.880000000000001"/>
-    <col customWidth="1" min="8" max="11" style="1" width="11.5"/>
+    <col customWidth="1" min="7" max="7" style="1" width="12.24"/>
+    <col customWidth="1" min="8" max="8" style="1" width="12"/>
+    <col customWidth="1" min="9" max="9" style="1" width="12.880000000000001"/>
+    <col customWidth="1" min="10" max="13" style="1" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -3131,10 +3233,10 @@
       <c r="C1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>147</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -3146,67 +3248,81 @@
       <c r="H1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>153</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+        <v>158</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
-      <c r="K2" s="14">
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+        <v>183</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="14">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="14">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3214,26 +3330,30 @@
       <c r="A4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>195</v>
+      <c r="B4" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
+        <v>186</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="14">
+      <c r="H4" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3241,53 +3361,61 @@
       <c r="A5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>184</v>
+      <c r="B5" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>0</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="14">
+        <v>166</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="E6" s="1"/>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
         <v>1</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="14">
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3296,25 +3424,29 @@
         <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>0</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14">
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3323,25 +3455,29 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>0</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+        <v>164</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="14">
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3350,25 +3486,29 @@
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+        <v>176</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="14">
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3377,25 +3517,29 @@
         <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+        <v>164</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="14">
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3441,45 +3585,45 @@
         <v>145</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>203</v>
+        <v>147</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" ht="13.5">
       <c r="A2" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22">
@@ -3499,13 +3643,13 @@
         <v>135</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C3" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>204</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22">
@@ -3526,13 +3670,13 @@
         <v>134</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="F4" s="22">
         <v>0</v>
@@ -3555,7 +3699,7 @@
         <v>206</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>207</v>
@@ -3581,7 +3725,7 @@
         <v>210</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>207</v>
@@ -3617,7 +3761,7 @@
         <v>214</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>207</v>

</xml_diff>

<commit_message>
RAB-1823: update source file xlsx & expected batteries accondingly
</commit_message>
<xml_diff>
--- a/tests/Command/GenerateTemplatesCommand/source_file.xlsx
+++ b/tests/Command/GenerateTemplatesCommand/source_file.xlsx
@@ -4,16 +4,17 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Industries" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="attribute_options" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="families_descriptions" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="videogames" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="headphones" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="jerseys" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="batteries" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="attribute_groups" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="families_descriptions" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="videogames" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="headphones" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="jerseys" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="batteries" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
@@ -494,6 +495,18 @@
     <t>Oversized</t>
   </si>
   <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>dpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPP (Digital Product Passport)</t>
+  </si>
+  <si>
     <t>attribute_as_main_media</t>
   </si>
   <si>
@@ -584,9 +597,6 @@
     <t>pim_catalog_identifier</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>template</t>
   </si>
   <si>
@@ -722,83 +732,74 @@
     <t>Cut</t>
   </si>
   <si>
+    <t>battery_passport_identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery passport identification</t>
+  </si>
+  <si>
+    <t>responsible_economic_operator_identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsible economic operator identification</t>
+  </si>
+  <si>
+    <t>pim_catalog_number</t>
+  </si>
+  <si>
+    <t>manufacturers_identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer's identification</t>
+  </si>
+  <si>
+    <t>manufacturing_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing date</t>
+  </si>
+  <si>
+    <t>pim_catalog_date</t>
+  </si>
+  <si>
+    <t>manufacturing_place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturing place</t>
+  </si>
+  <si>
+    <t>battery_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery category</t>
+  </si>
+  <si>
+    <t>battery_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery weight</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>GRAM</t>
+  </si>
+  <si>
     <t>eu_declaration_of_conformity</t>
   </si>
   <si>
     <t xml:space="preserve">EU declaration of conformity</t>
   </si>
   <si>
-    <t>dpp</t>
-  </si>
-  <si>
     <t>url</t>
-  </si>
-  <si>
-    <t>original_power_capability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Original power capability (in Watts)</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>WATT</t>
-  </si>
-  <si>
-    <t>maximum_permitted_battery_power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum permitted battery power</t>
-  </si>
-  <si>
-    <t>ratio_between_nominal_allowed_battery_power_and_battery_energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio between nominal allowed battery power (W) and battery energy (Wh)</t>
-  </si>
-  <si>
-    <t>pim_catalog_number</t>
-  </si>
-  <si>
-    <t>initial_round_trip_energy_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial round trip energy efficiency</t>
-  </si>
-  <si>
-    <t>round_trip_energy_efficiency_at_50_percent_of_cycle_life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round trip energy efficiency at 50% of cycle life</t>
-  </si>
-  <si>
-    <t>date_of_putting_the_battery_into_service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of putting the battery into service</t>
-  </si>
-  <si>
-    <t>pim_catalog_date</t>
-  </si>
-  <si>
-    <t>temperature_range_idle_state_lower_boundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature range idle state (lower boundary)</t>
-  </si>
-  <si>
-    <t>temperature_range_idle_state_upper_boundary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature range idle state (upper boundary)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -819,45 +820,59 @@
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="10.000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.000000"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color indexed="64"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -879,7 +894,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -897,11 +912,14 @@
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
@@ -918,9 +936,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -943,12 +958,15 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
     <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
     <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+    <xf fontId="10" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="9" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0"/>
+    <xf fontId="10" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="0"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -972,7 +990,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName=" " id="{BC36CD6E-B780-8099-B33A-D6EAA0A89997}"/>
+  <person displayName=" " id="{0C4A97D7-E58E-BCCA-6314-898E8927E571}"/>
 </personList>
 </file>
 
@@ -1432,7 +1450,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" personId="{BC36CD6E-B780-8099-B33A-D6EAA0A89997}" id="{00190023-0011-4759-8904-001F003A0020}" done="0">
+  <threadedComment ref="A1" personId="{0C4A97D7-E58E-BCCA-6314-898E8927E571}" id="{00190023-0011-4759-8904-001F003A0020}" done="0">
     <text xml:space="preserve">Tires are so complicated. Variant are under at least 3 levels of variation "height, width, diameter, charge indice". It is a pitfall here.
 -Nelly Devaine
 ----
@@ -2217,6 +2235,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
@@ -2235,88 +2294,88 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>130</v>
+      <c r="C1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>134</v>
+      <c r="A2" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>143</v>
+      <c r="E4" s="12" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>144</v>
+        <v>139</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2327,7 +2386,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3" disablePrompts="0">
-        <x14:dataValidation xr:uid="{004F0023-0092-4041-B8C8-006C00A600E5}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="_x0001_" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00470031-00A9-4DFE-AD3A-007500360011}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="_x0001_" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(#ref!)&lt;255</xm:f>
           </x14:formula1>
@@ -2336,13 +2395,13 @@
           </x14:formula2>
           <xm:sqref>E2:E4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{000400A8-004B-4CFD-A5A3-004B001C000F}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00990077-00AB-42DE-9903-00740060002F}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(C16)&lt;255</xm:f>
           </x14:formula1>
           <xm:sqref>C5:D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00B70015-0050-47AE-919B-008800DA00AB}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00C800FF-00B0-4C75-9F82-002E00AF0027}" type="custom" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" prompt="255 characters max allowed" showDropDown="1" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>LEN(B16)&lt;255</xm:f>
           </x14:formula1>
@@ -2354,7 +2413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
@@ -2384,98 +2443,98 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="13">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15">
+      <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>161</v>
+        <v>139</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="13">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13">
+      <c r="F3" s="15">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15">
         <v>1</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="13">
+      <c r="H3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2483,127 +2542,127 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="13">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>165</v>
+        <v>138</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="13">
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>168</v>
+        <v>170</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="13">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="13">
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="13">
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2611,30 +2670,30 @@
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>175</v>
+      <c r="B8" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="13">
+      <c r="F8" s="15">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2642,30 +2701,30 @@
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>177</v>
+      <c r="B9" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="13">
+      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2673,30 +2732,30 @@
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>178</v>
+      <c r="B10" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="13">
+      <c r="F10" s="15">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2704,30 +2763,30 @@
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="13">
+      <c r="F11" s="15">
+        <v>0</v>
+      </c>
+      <c r="G11" s="15">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2735,55 +2794,55 @@
       <c r="A12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>180</v>
+      <c r="B12" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="13">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>160</v>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="13">
+      <c r="M12" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="13" ht="12.800000000000001">
       <c r="A13" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="13">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>160</v>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="K13" s="1">
         <v>1</v>
@@ -2803,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
@@ -2833,362 +2892,362 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="D1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="E1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>152</v>
       </c>
+      <c r="G1" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>156</v>
+      </c>
       <c r="K1" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14">
+      <c r="F2" s="16">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>182</v>
+        <v>184</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="14">
-        <v>0</v>
-      </c>
-      <c r="G3" s="14">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14">
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>161</v>
+        <v>139</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
         <v>1</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14">
+      <c r="H4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>185</v>
+        <v>187</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="14">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="14">
+      <c r="H5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>165</v>
+        <v>138</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14">
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>187</v>
+        <v>142</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="14">
-        <v>0</v>
-      </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="14">
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="14">
-        <v>0</v>
-      </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="16">
         <v>1</v>
       </c>
-      <c r="L8" s="14">
-        <v>0</v>
-      </c>
-      <c r="M8" s="14">
+      <c r="L8" s="16">
+        <v>0</v>
+      </c>
+      <c r="M8" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="14">
-        <v>0</v>
-      </c>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" s="14">
+      <c r="J9" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" s="16">
         <v>1</v>
       </c>
-      <c r="L9" s="14">
-        <v>0</v>
-      </c>
-      <c r="M9" s="14">
+      <c r="L9" s="16">
+        <v>0</v>
+      </c>
+      <c r="M9" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="14">
-        <v>0</v>
-      </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14">
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="14">
-        <v>0</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14">
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3200,7 +3259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
@@ -3231,191 +3290,191 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14">
+      <c r="F2" s="16">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>182</v>
+        <v>184</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="14">
-        <v>0</v>
-      </c>
-      <c r="G3" s="14">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14">
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>198</v>
+        <v>143</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
         <v>1</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="14">
+      <c r="H4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>187</v>
+        <v>142</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="14">
-        <v>0</v>
-      </c>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="14">
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="14">
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
         <v>1</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14">
+      <c r="H6" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3424,29 +3483,29 @@
         <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="14">
-        <v>0</v>
-      </c>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14">
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3455,29 +3514,29 @@
         <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="14">
-        <v>0</v>
-      </c>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="14">
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3486,29 +3545,29 @@
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="14">
-        <v>0</v>
-      </c>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14">
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3517,29 +3576,29 @@
         <v>122</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="14">
-        <v>0</v>
-      </c>
-      <c r="G10" s="14">
-        <v>0</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14">
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16">
         <v>0</v>
       </c>
     </row>
@@ -3554,10 +3613,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="DN135" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3575,433 +3634,409 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="D1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="F1" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="G1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="K1" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="18" t="s">
+      <c r="H1" s="7" t="s">
         <v>155</v>
       </c>
+      <c r="I1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="2" ht="13.5">
-      <c r="A2" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22">
-        <v>0</v>
-      </c>
-      <c r="G2" s="22">
-        <v>0</v>
-      </c>
-      <c r="I2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22">
+      <c r="A2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2" s="8"/>
+      <c r="J2"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="13.5">
-      <c r="A3" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="A3" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5">
+      <c r="A4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4"/>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5">
+      <c r="A5" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="22">
+      <c r="D5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" s="8">
         <v>1</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" ht="13.5">
-      <c r="A4" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    </row>
+    <row r="6" ht="13.5">
+      <c r="A6" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="13.5">
+      <c r="A7" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" s="8">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" ht="13.5">
+      <c r="A8" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" ht="13.5">
+      <c r="A9" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22">
-        <v>0</v>
-      </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="L4" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" ht="13.5">
-      <c r="A5" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
+      <c r="D9" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
         <v>1</v>
       </c>
-      <c r="L5" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="13.5">
-      <c r="A6" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="J6" s="22">
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" ht="13.5">
+      <c r="A10" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" ht="13.5">
+      <c r="A11" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="J11" s="8">
         <v>1</v>
       </c>
-      <c r="K6" s="22">
-        <v>0</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="13.5">
-      <c r="A7" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22">
-        <v>0</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="J7" s="22">
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" ht="13.5">
+      <c r="A12" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="22">
-        <v>0</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="13.5">
-      <c r="A8" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22">
-        <v>0</v>
-      </c>
-      <c r="G8" s="22">
-        <v>0</v>
-      </c>
-      <c r="J8" s="22">
-        <v>0</v>
-      </c>
-      <c r="K8" s="22">
-        <v>1</v>
-      </c>
-      <c r="L8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="13.5">
-      <c r="A9" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
-      <c r="G9" s="22">
-        <v>0</v>
-      </c>
-      <c r="J9" s="22">
-        <v>0</v>
-      </c>
-      <c r="K9" s="22">
-        <v>1</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" ht="13.5">
-      <c r="A10" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
-        <v>0</v>
-      </c>
-      <c r="G10" s="22">
-        <v>0</v>
-      </c>
-      <c r="J10" s="22">
-        <v>0</v>
-      </c>
-      <c r="K10" s="22">
-        <v>1</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="13.5">
-      <c r="A11" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22">
-        <v>0</v>
-      </c>
-      <c r="G11" s="22">
-        <v>0</v>
-      </c>
-      <c r="L11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="13.5">
-      <c r="A12" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22">
-        <v>0</v>
-      </c>
-      <c r="G12" s="22">
-        <v>0</v>
-      </c>
-      <c r="J12" s="22">
-        <v>0</v>
-      </c>
-      <c r="K12" s="22">
-        <v>1</v>
-      </c>
-      <c r="L12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="13.5">
-      <c r="A13" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22">
-        <v>0</v>
-      </c>
-      <c r="G13" s="22">
-        <v>0</v>
-      </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="22">
-        <v>1</v>
-      </c>
-      <c r="L13" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75"/>
+    <row r="14" ht="12.75"/>
+    <row r="15" ht="12.75"/>
+    <row r="16" ht="12.75"/>
+    <row r="17" ht="12.75"/>
+    <row r="18" ht="12.75"/>
+    <row r="19" ht="12.75"/>
+    <row r="20" ht="12.75"/>
+    <row r="21" ht="12.75"/>
+    <row r="22" ht="12.75"/>
+    <row r="23" ht="12.75"/>
+    <row r="24" ht="12.75"/>
+    <row r="25" ht="12.75"/>
+    <row r="26" ht="12.75"/>
+    <row r="27" ht="12.75"/>
+    <row r="28" ht="12.75"/>
+    <row r="29" ht="12.75"/>
+    <row r="30" ht="12.75"/>
+    <row r="31" ht="12.75"/>
+    <row r="32" ht="12.75"/>
+    <row r="33" ht="12.75"/>
+    <row r="34" ht="12.75"/>
+    <row r="35" ht="12.75"/>
+    <row r="36" ht="12.75"/>
+    <row r="37" ht="12.75"/>
+    <row r="38" ht="12.75"/>
+    <row r="39" ht="12.75"/>
+    <row r="40" ht="12.75"/>
+    <row r="41" ht="12.75"/>
+    <row r="42" ht="12.75"/>
+    <row r="43" ht="12.75"/>
+    <row r="44" ht="12.75"/>
+    <row r="45" ht="12.75"/>
+    <row r="46" ht="12.75"/>
+    <row r="47" ht="12.75"/>
+    <row r="48" ht="12.75"/>
+    <row r="49" ht="12.75"/>
+    <row r="50" ht="12.75"/>
+    <row r="51" ht="12.75"/>
+    <row r="52" ht="12.75"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>